<commit_message>
parser: bad fit: OOP version:Goley filter
</commit_message>
<xml_diff>
--- a/DC/tektronix_parser.xlsx
+++ b/DC/tektronix_parser.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="295k" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>T</t>
   </si>
@@ -34,6 +34,63 @@
   </si>
   <si>
     <t>dDC</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>f2_bad</t>
+  </si>
+  <si>
+    <t>f3_bad</t>
+  </si>
+  <si>
+    <t>chi2_per_dof_th</t>
+  </si>
+  <si>
+    <t>f1_good</t>
+  </si>
+  <si>
+    <t>f1_bad</t>
+  </si>
+  <si>
+    <t>шумы</t>
+  </si>
+  <si>
+    <t>одиночные</t>
+  </si>
+  <si>
+    <t>двойные</t>
+  </si>
+  <si>
+    <t>тройные</t>
+  </si>
+  <si>
+    <t>f2_good</t>
+  </si>
+  <si>
+    <t>всего</t>
+  </si>
+  <si>
+    <t>f3_good</t>
+  </si>
+  <si>
+    <t>одиночное, принятое за 2-е</t>
+  </si>
+  <si>
+    <t>двойных</t>
+  </si>
+  <si>
+    <t>тройных</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> одиночных</t>
+  </si>
+  <si>
+    <t>правильное нахождение</t>
+  </si>
+  <si>
+    <t>количество</t>
   </si>
 </sst>
 </file>
@@ -72,11 +129,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1342,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,1229 +1627,486 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>681.42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>710.86</v>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2">
-        <f>A2-A1</f>
-        <v>29.440000000000055</v>
+        <v>72</v>
       </c>
       <c r="C2">
-        <v>2.4686099999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>770.43600000000004</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B66" si="0">A3-A2</f>
-        <v>59.576000000000022</v>
+        <v>51</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>6.5145400000000006E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1024.55</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>254.11399999999992</v>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>3.6211300000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1103.8800000000001</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>79.330000000000155</v>
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>3.9619599999999998E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1189.77</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>85.889999999999873</v>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>3.9999300000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1431.41</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>241.6400000000001</v>
-      </c>
-      <c r="C7">
-        <v>3.78591E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1562.72</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>131.30999999999995</v>
-      </c>
-      <c r="C8">
-        <v>0.19580700000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1578.86</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>16.139999999999873</v>
-      </c>
-      <c r="C9">
-        <v>4.3330300000000002E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1663.97</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>85.110000000000127</v>
-      </c>
-      <c r="C10">
-        <v>8.8248499999999994E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1678.51</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>14.539999999999964</v>
-      </c>
-      <c r="C11">
-        <v>6.5688399999999994E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2735.52</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>1057.01</v>
-      </c>
-      <c r="C12">
-        <v>4.3470399999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3058.23</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>322.71000000000004</v>
-      </c>
-      <c r="C13">
-        <v>4.7851499999999998E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>3259.94</v>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>1261/398</f>
+        <v>3.1683417085427137</v>
+      </c>
+      <c r="G9">
+        <f>5313/398</f>
+        <v>13.349246231155778</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>1619/499</f>
+        <v>3.2444889779559118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f>1413/461</f>
+        <v>3.0650759219088939</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>201.71000000000004</v>
+        <v>72</v>
       </c>
       <c r="C14">
-        <v>3.6109299999999997E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3991.19</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>731.25</v>
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>6.8893399999999994E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4033.76</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>42.570000000000164</v>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
       </c>
       <c r="C16">
-        <v>3.8124600000000002E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4485.54</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>451.77999999999975</v>
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>3.9897700000000001E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4965.1000000000004</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>479.5600000000004</v>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
       </c>
       <c r="C18">
-        <v>4.2364400000000003E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5741.36</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>776.25999999999931</v>
-      </c>
-      <c r="C19">
-        <v>4.4149500000000001E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>6052.4</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>311.03999999999996</v>
-      </c>
-      <c r="C20">
-        <v>4.5255499999999997E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6189.76</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>137.36000000000058</v>
-      </c>
-      <c r="C21">
-        <v>6.4393099999999995E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>6491.66</v>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
-        <v>301.89999999999964</v>
+        <v>72</v>
       </c>
       <c r="C22">
-        <v>3.80442E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>6610.28</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>118.61999999999989</v>
+        <v>54</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="4">
+        <f>C24/(C24+C23)</f>
+        <v>0.98148148148148151</v>
+      </c>
+      <c r="M22" s="4">
+        <f>E25/(E25 + F25)</f>
+        <v>0.9</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>8.6562700000000006E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6620.4</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>10.119999999999891</v>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="4">
+        <f>C24/B22</f>
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="M23" s="4">
+        <f>D25/B22</f>
+        <v>0.15277777777777779</v>
+      </c>
+      <c r="N23" s="4">
+        <f>D26/B22</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>7.4535799999999999E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>6833.85</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>213.45000000000073</v>
+        <v>53</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
       </c>
       <c r="C25">
-        <v>6.3094999999999998E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>7003.04</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>169.1899999999996</v>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>4.4065199999999999E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>7290.57</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>287.52999999999975</v>
-      </c>
-      <c r="C27">
-        <v>3.6352799999999998E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>7439.11</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>148.53999999999996</v>
-      </c>
-      <c r="C28">
-        <v>4.6818800000000001E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>7459.88</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>20.770000000000437</v>
-      </c>
-      <c r="C29">
-        <v>7.4091799999999999E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>7494.43</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>34.550000000000182</v>
-      </c>
-      <c r="C30">
-        <v>6.4664899999999997E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>7806.66</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>312.22999999999956</v>
-      </c>
-      <c r="C31">
-        <v>4.3021499999999997E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>7959.53</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>152.86999999999989</v>
-      </c>
-      <c r="C32">
-        <v>4.70572E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>7984.48</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>24.949999999999818</v>
-      </c>
-      <c r="C33">
-        <v>3.6252100000000002E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>7984.59</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>0.11000000000058208</v>
-      </c>
-      <c r="C34">
-        <v>0.181945</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>8075.6</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>91.010000000000218</v>
-      </c>
-      <c r="C35">
-        <v>285.49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>8084.45</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>8.8499999999994543</v>
-      </c>
-      <c r="C36">
-        <v>3.7908299999999999E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>8127.42</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>42.970000000000255</v>
-      </c>
-      <c r="C37">
-        <v>5.7712199999999998E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>8254.68</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>127.26000000000022</v>
-      </c>
-      <c r="C38">
-        <v>3.67192E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>8335.08</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>80.399999999999636</v>
-      </c>
-      <c r="C39">
-        <v>4.4758199999999998E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>8379.76</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>44.680000000000291</v>
-      </c>
-      <c r="C40">
-        <v>6.34266E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>8608.74</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>228.97999999999956</v>
-      </c>
-      <c r="C41">
-        <v>5.2039799999999997E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>8628.26</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="0"/>
-        <v>19.520000000000437</v>
-      </c>
-      <c r="C42">
-        <v>9.7429199999999994E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>8885.02</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="0"/>
-        <v>256.76000000000022</v>
-      </c>
-      <c r="C43">
-        <v>4.4828199999999999E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>8906.4599999999991</v>
-      </c>
-      <c r="B44">
-        <f t="shared" si="0"/>
-        <v>21.43999999999869</v>
-      </c>
-      <c r="C44">
-        <v>3.6571600000000003E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>8928.1299999999992</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="0"/>
-        <v>21.670000000000073</v>
-      </c>
-      <c r="C45">
-        <v>4.4619100000000002E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>9185.34</v>
-      </c>
-      <c r="B46">
-        <f t="shared" si="0"/>
-        <v>257.21000000000095</v>
-      </c>
-      <c r="C46">
-        <v>0.12654699999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>9257.48</v>
-      </c>
-      <c r="B47">
-        <f t="shared" si="0"/>
-        <v>72.139999999999418</v>
-      </c>
-      <c r="C47">
-        <v>4.79867E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>9525.5300000000007</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="0"/>
-        <v>268.05000000000109</v>
-      </c>
-      <c r="C48">
-        <v>4.57761E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>9793.9699999999993</v>
-      </c>
-      <c r="B49">
-        <f t="shared" si="0"/>
-        <v>268.43999999999869</v>
-      </c>
-      <c r="C49">
-        <v>4.40807E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>9845.24</v>
-      </c>
-      <c r="B50">
-        <f t="shared" si="0"/>
-        <v>51.270000000000437</v>
-      </c>
-      <c r="C50">
-        <v>8.2582900000000001E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>9861</v>
-      </c>
-      <c r="B51">
-        <f t="shared" si="0"/>
-        <v>15.760000000000218</v>
-      </c>
-      <c r="C51">
-        <v>3.60592E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>10839.9</v>
-      </c>
-      <c r="B52">
-        <f t="shared" si="0"/>
-        <v>978.89999999999964</v>
-      </c>
-      <c r="C52">
-        <v>4.5393500000000003E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>10850.1</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="0"/>
-        <v>10.200000000000728</v>
-      </c>
-      <c r="C53">
-        <v>3.2339100000000003E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>10993</v>
-      </c>
-      <c r="B54">
-        <f t="shared" si="0"/>
-        <v>142.89999999999964</v>
-      </c>
-      <c r="C54">
-        <v>6.9942299999999999E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>11203.3</v>
-      </c>
-      <c r="B55">
-        <f t="shared" si="0"/>
-        <v>210.29999999999927</v>
-      </c>
-      <c r="C55">
-        <v>4.3353900000000001E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>11306.1</v>
-      </c>
-      <c r="B56">
-        <f t="shared" si="0"/>
-        <v>102.80000000000109</v>
-      </c>
-      <c r="C56">
-        <v>4.2178800000000002E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>11428.4</v>
-      </c>
-      <c r="B57">
-        <f t="shared" si="0"/>
-        <v>122.29999999999927</v>
-      </c>
-      <c r="C57">
-        <v>4.7144600000000002E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>11519.5</v>
-      </c>
-      <c r="B58">
-        <f t="shared" si="0"/>
-        <v>91.100000000000364</v>
-      </c>
-      <c r="C58">
-        <v>4.4548900000000002E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>11824</v>
-      </c>
-      <c r="B59">
-        <f t="shared" si="0"/>
-        <v>304.5</v>
-      </c>
-      <c r="C59">
-        <v>5.7886E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>11865.5</v>
-      </c>
-      <c r="B60">
-        <f t="shared" si="0"/>
-        <v>41.5</v>
-      </c>
-      <c r="C60">
-        <v>3.9417800000000003E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>12066.4</v>
-      </c>
-      <c r="B61">
-        <f t="shared" si="0"/>
-        <v>200.89999999999964</v>
-      </c>
-      <c r="C61">
-        <v>6.0337300000000003E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>12338</v>
-      </c>
-      <c r="B62">
-        <f t="shared" si="0"/>
-        <v>271.60000000000036</v>
-      </c>
-      <c r="C62">
-        <v>3.9763100000000003E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>12591.1</v>
-      </c>
-      <c r="B63">
-        <f t="shared" si="0"/>
-        <v>253.10000000000036</v>
-      </c>
-      <c r="C63">
-        <v>4.57452E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>12603.7</v>
-      </c>
-      <c r="B64">
-        <f t="shared" si="0"/>
-        <v>12.600000000000364</v>
-      </c>
-      <c r="C64">
-        <v>0.107969</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>12625.9</v>
-      </c>
-      <c r="B65">
-        <f t="shared" si="0"/>
-        <v>22.199999999998909</v>
-      </c>
-      <c r="C65">
-        <v>0.1419</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>13589.1</v>
-      </c>
-      <c r="B66">
-        <f t="shared" si="0"/>
-        <v>963.20000000000073</v>
-      </c>
-      <c r="C66">
-        <v>4.34224E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>13796.5</v>
-      </c>
-      <c r="B67">
-        <f t="shared" ref="B67:B102" si="1">A67-A66</f>
-        <v>207.39999999999964</v>
-      </c>
-      <c r="C67">
-        <v>4.7560699999999997E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>13797.4</v>
-      </c>
-      <c r="B68">
-        <f t="shared" si="1"/>
-        <v>0.8999999999996362</v>
-      </c>
-      <c r="C68">
-        <v>4.1923099999999998E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>13804.4</v>
-      </c>
-      <c r="B69">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>7</v>
       </c>
-      <c r="C69">
-        <v>7.7926700000000002E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>13933.7</v>
-      </c>
-      <c r="B70">
-        <f t="shared" si="1"/>
-        <v>129.30000000000109</v>
-      </c>
-      <c r="C70">
-        <v>4.7829799999999999E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>13936.7</v>
-      </c>
-      <c r="B71">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="C71">
-        <v>6.7737500000000006E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>13944.7</v>
-      </c>
-      <c r="B72">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C72">
-        <v>4.90646E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>14008</v>
-      </c>
-      <c r="B73">
-        <f t="shared" si="1"/>
-        <v>63.299999999999272</v>
-      </c>
-      <c r="C73">
-        <v>4.1995499999999998E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>14154.9</v>
-      </c>
-      <c r="B74">
-        <f t="shared" si="1"/>
-        <v>146.89999999999964</v>
-      </c>
-      <c r="C74">
-        <v>0.12255000000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>14175.7</v>
-      </c>
-      <c r="B75">
-        <f t="shared" si="1"/>
-        <v>20.800000000001091</v>
-      </c>
-      <c r="C75">
-        <v>3.9580499999999998E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>14263.8</v>
-      </c>
-      <c r="B76">
-        <f t="shared" si="1"/>
-        <v>88.099999999998545</v>
-      </c>
-      <c r="C76">
-        <v>6.1205000000000002E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>14357.8</v>
-      </c>
-      <c r="B77">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="C77">
-        <v>7.8686000000000006E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>14412.6</v>
-      </c>
-      <c r="B78">
-        <f t="shared" si="1"/>
-        <v>54.800000000001091</v>
-      </c>
-      <c r="C78">
-        <v>4.46188E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>15192.9</v>
-      </c>
-      <c r="B79">
-        <f t="shared" si="1"/>
-        <v>780.29999999999927</v>
-      </c>
-      <c r="C79">
-        <v>6.5145300000000003E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>15233.2</v>
-      </c>
-      <c r="B80">
-        <f t="shared" si="1"/>
-        <v>40.300000000001091</v>
-      </c>
-      <c r="C80">
-        <v>2.2113600000000001E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>15244.2</v>
-      </c>
-      <c r="B81">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="C81">
-        <v>6.2879599999999994E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>15355.5</v>
-      </c>
-      <c r="B82">
-        <f t="shared" si="1"/>
-        <v>111.29999999999927</v>
-      </c>
-      <c r="C82">
-        <v>3.7708600000000002E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>15458.4</v>
-      </c>
-      <c r="B83">
-        <f t="shared" si="1"/>
-        <v>102.89999999999964</v>
-      </c>
-      <c r="C83">
-        <v>5.0087899999999998E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>15488.7</v>
-      </c>
-      <c r="B84">
-        <f t="shared" si="1"/>
-        <v>30.300000000001091</v>
-      </c>
-      <c r="C84">
-        <v>4.5751600000000003E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>15605.2</v>
-      </c>
-      <c r="B85">
-        <f t="shared" si="1"/>
-        <v>116.5</v>
-      </c>
-      <c r="C85">
-        <v>4.5012499999999997E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>15827.6</v>
-      </c>
-      <c r="B86">
-        <f t="shared" si="1"/>
-        <v>222.39999999999964</v>
-      </c>
-      <c r="C86">
-        <v>4.1657100000000002E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>16457.7</v>
-      </c>
-      <c r="B87">
-        <f t="shared" si="1"/>
-        <v>630.10000000000036</v>
-      </c>
-      <c r="C87">
-        <v>4.2596099999999998E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>16776</v>
-      </c>
-      <c r="B88">
-        <f t="shared" si="1"/>
-        <v>318.29999999999927</v>
-      </c>
-      <c r="C88">
-        <v>4.8952900000000001E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>16790.8</v>
-      </c>
-      <c r="B89">
-        <f t="shared" si="1"/>
-        <v>14.799999999999272</v>
-      </c>
-      <c r="C89">
-        <v>3.98149E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>17083.900000000001</v>
-      </c>
-      <c r="B90">
-        <f t="shared" si="1"/>
-        <v>293.10000000000218</v>
-      </c>
-      <c r="C90">
-        <v>4.7013699999999999E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>17479.3</v>
-      </c>
-      <c r="B91">
-        <f t="shared" si="1"/>
-        <v>395.39999999999782</v>
-      </c>
-      <c r="C91">
-        <v>4.4469300000000003E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>17748.5</v>
-      </c>
-      <c r="B92">
-        <f t="shared" si="1"/>
-        <v>269.20000000000073</v>
-      </c>
-      <c r="C92">
-        <v>5.6014099999999997E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>17811</v>
-      </c>
-      <c r="B93">
-        <f t="shared" si="1"/>
-        <v>62.5</v>
-      </c>
-      <c r="C93">
-        <v>4.03875E-2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>18091.2</v>
-      </c>
-      <c r="B94">
-        <f t="shared" si="1"/>
-        <v>280.20000000000073</v>
-      </c>
-      <c r="C94">
-        <v>4.33119E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>18704.400000000001</v>
-      </c>
-      <c r="B95">
-        <f t="shared" si="1"/>
-        <v>613.20000000000073</v>
-      </c>
-      <c r="C95">
-        <v>2.17065E-2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>18713.7</v>
-      </c>
-      <c r="B96">
-        <f t="shared" si="1"/>
-        <v>9.2999999999992724</v>
-      </c>
-      <c r="C96">
-        <v>0.105175</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>18714.900000000001</v>
-      </c>
-      <c r="B97">
-        <f t="shared" si="1"/>
-        <v>1.2000000000007276</v>
-      </c>
-      <c r="C97">
-        <v>1.8049800000000001E-2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>18795</v>
-      </c>
-      <c r="B98">
-        <f t="shared" si="1"/>
-        <v>80.099999999998545</v>
-      </c>
-      <c r="C98">
-        <v>4.1272099999999999E-2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>18876.8</v>
-      </c>
-      <c r="B99">
-        <f t="shared" si="1"/>
-        <v>81.799999999999272</v>
-      </c>
-      <c r="C99">
-        <v>4.1744999999999997E-2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>19005.900000000001</v>
-      </c>
-      <c r="B100">
-        <f t="shared" si="1"/>
-        <v>129.10000000000218</v>
-      </c>
-      <c r="C100">
-        <v>0.101578</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>19717.599999999999</v>
-      </c>
-      <c r="B101">
-        <f t="shared" si="1"/>
-        <v>711.69999999999709</v>
-      </c>
-      <c r="C101">
-        <v>4.0402599999999997E-2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>19838.8</v>
-      </c>
-      <c r="B102">
-        <f t="shared" si="1"/>
-        <v>121.20000000000073</v>
-      </c>
-      <c r="C102">
-        <v>4.01293E-2</v>
+      <c r="G26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parser: add time front graph
</commit_message>
<xml_diff>
--- a/DC/tektronix_parser.xlsx
+++ b/DC/tektronix_parser.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t>T</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>количество</t>
+  </si>
+  <si>
+    <t>golay filter</t>
   </si>
 </sst>
 </file>
@@ -1627,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,6 +2112,90 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30">
+        <v>79</v>
+      </c>
+      <c r="D30">
+        <v>19</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
parser: unit tests work
</commit_message>
<xml_diff>
--- a/DC/tektronix_parser.xlsx
+++ b/DC/tektronix_parser.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
   <si>
     <t>T</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>количество</t>
-  </si>
-  <si>
-    <t>golay filter</t>
   </si>
 </sst>
 </file>
@@ -1630,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,9 +2134,6 @@
       <c r="J29" t="s">
         <v>9</v>
       </c>
-      <c r="K29" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2177,7 +2171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2185,7 +2179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2194,6 +2188,60 @@
       </c>
       <c r="F34">
         <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parser: good fit 3 signal
</commit_message>
<xml_diff>
--- a/DC/tektronix_parser.xlsx
+++ b/DC/tektronix_parser.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
   <si>
     <t>T</t>
   </si>
@@ -1627,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2220,6 +2220,21 @@
       <c r="A38" t="s">
         <v>17</v>
       </c>
+      <c r="B38">
+        <v>78</v>
+      </c>
+      <c r="C38">
+        <v>58</v>
+      </c>
+      <c r="D38">
+        <v>20</v>
+      </c>
+      <c r="E38">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>9</v>
+      </c>
       <c r="J38">
         <v>5</v>
       </c>
@@ -2228,19 +2243,139 @@
       <c r="A39" t="s">
         <v>12</v>
       </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
+      <c r="C40">
+        <v>49</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <v>9</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46">
+        <v>78</v>
+      </c>
+      <c r="C46">
+        <v>58</v>
+      </c>
+      <c r="D46">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parser: strange errors with Math funvtions
</commit_message>
<xml_diff>
--- a/DC/tektronix_parser.xlsx
+++ b/DC/tektronix_parser.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="295k" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="test_signal" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="30">
   <si>
     <t>T</t>
   </si>
@@ -91,6 +92,21 @@
   </si>
   <si>
     <t>количество</t>
+  </si>
+  <si>
+    <t>tau ns</t>
+  </si>
+  <si>
+    <t>f4_good</t>
+  </si>
+  <si>
+    <t>f4_bad</t>
+  </si>
+  <si>
+    <t>f5_good</t>
+  </si>
+  <si>
+    <t>f5_bad</t>
   </si>
 </sst>
 </file>
@@ -1629,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,4 +2580,278 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>39</v>
+      </c>
+      <c r="C2">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>1080</v>
+      </c>
+      <c r="C14">
+        <v>604</v>
+      </c>
+      <c r="E14">
+        <v>258</v>
+      </c>
+      <c r="G14">
+        <v>133</v>
+      </c>
+      <c r="I14">
+        <v>52</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+      <c r="N14">
+        <f>SUM(C14:K14)/B14</f>
+        <v>0.98796296296296293</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1080</v>
+      </c>
+      <c r="C15">
+        <v>596</v>
+      </c>
+      <c r="E15">
+        <v>246</v>
+      </c>
+      <c r="G15">
+        <v>134</v>
+      </c>
+      <c r="I15">
+        <v>53</v>
+      </c>
+      <c r="K15">
+        <v>29</v>
+      </c>
+      <c r="N15">
+        <f>SUM(C15:K15)/B15</f>
+        <v>0.97962962962962963</v>
+      </c>
+      <c r="O15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1080</v>
+      </c>
+      <c r="C16">
+        <v>576</v>
+      </c>
+      <c r="E16">
+        <v>234</v>
+      </c>
+      <c r="G16">
+        <v>128</v>
+      </c>
+      <c r="I16">
+        <v>61</v>
+      </c>
+      <c r="K16">
+        <v>41</v>
+      </c>
+      <c r="N16">
+        <f>SUM(C16:K16)/B16</f>
+        <v>0.96296296296296291</v>
+      </c>
+      <c r="O16">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
parser: stable, but bad fit in simulation 2
</commit_message>
<xml_diff>
--- a/DC/tektronix_parser.xlsx
+++ b/DC/tektronix_parser.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="295k" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="test_signal" sheetId="4" r:id="rId4"/>
+    <sheet name="Лист5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="35">
   <si>
     <t>T</t>
   </si>
@@ -107,6 +108,21 @@
   </si>
   <si>
     <t>f5_bad</t>
+  </si>
+  <si>
+    <t>tau rec</t>
+  </si>
+  <si>
+    <t>tau ap</t>
+  </si>
+  <si>
+    <t>f_ksi</t>
+  </si>
+  <si>
+    <t>ksi</t>
+  </si>
+  <si>
+    <t>tau rec / tau ap</t>
   </si>
 </sst>
 </file>
@@ -536,7 +552,389 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист5!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист5!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39155606413637217</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.458498938424592</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54833698960847232</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67414953846125991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86071448389979044</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1606961092786015</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7066184472587207</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9383175078300776</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.4383895214284808</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>162.7342313896969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="427270640"/>
+        <c:axId val="427270248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="427270640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427270248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="427270248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427270640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1092,6 +1490,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1106,6 +2020,41 @@
       <xdr:colOff>147637</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2586,8 +3535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2854,4 +3803,149 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <f>A2/B2</f>
+        <v>0.34</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>$C$2 * EXP(- $C$2 * LN(1 - E2) ) / (1 - E2)</f>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <f>$C$2 * EXP(- $C$2 * LN(1 - E3) ) / (1 - E3)</f>
+        <v>0.39155606413637217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0.2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F7" si="0">$C$2 * EXP(- $C$2 * LN(1 - E4) ) / (1 - E4)</f>
+        <v>0.458498938424592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0.3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.54833698960847232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0.4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.67414953846125991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <f>$C$2 * EXP(- $C$2 * LN(1 - E7) ) / (1 - E7)</f>
+        <v>0.86071448389979044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F12" si="1">$C$2 * EXP(- $C$2 * LN(1 - E8) ) / (1 - E8)</f>
+        <v>1.1606961092786015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>0.7</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.7066184472587207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0.8</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.9383175078300776</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>0.9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>7.4383895214284808</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>0.99</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>162.7342313896969</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>